<commit_message>
Add all updated code
</commit_message>
<xml_diff>
--- a/PLFS_Metadata.xlsx
+++ b/PLFS_Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7AB0C9-530B-466F-A181-FEE026A39C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC56407-F692-41F4-B4B3-5EE7DFBE9EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90ACCF8D-C7D2-4D6D-9247-02748FDDC274}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="230">
   <si>
     <t>Andhra Pradesh</t>
   </si>
@@ -156,36 +156,15 @@
     <t>gender_code</t>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>Labour Force Participation Rate (LFPR)</t>
-  </si>
-  <si>
     <t>status_code</t>
   </si>
   <si>
     <t>indicator_code</t>
   </si>
   <si>
-    <t>Worker Population Ratio (WPR)</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>eduction_level</t>
   </si>
   <si>
-    <t>Unemployment Rate (UR)</t>
-  </si>
-  <si>
     <t>Percentage  distribution of usually working persons</t>
   </si>
   <si>
@@ -309,30 +288,9 @@
     <t xml:space="preserve">casual labour </t>
   </si>
   <si>
-    <t>Average wage/salary earnings (Rs. 0.00) per day from casual labour work other than public works</t>
-  </si>
-  <si>
     <t>Average gross earnings (Rs. 0.00) during last 30 days from self-employment among self-employed persons</t>
   </si>
   <si>
-    <t>average no. of days worked in a week (0.0) for person with broad status in employment in CWS</t>
-  </si>
-  <si>
-    <t>average no. of days actually worked in a week (0.0) for person with broad status in employment in CWS</t>
-  </si>
-  <si>
-    <t>average number of hours (0.0) actually worked per week considering all the economic activities performed during the week for person with broad status in employment in CWS</t>
-  </si>
-  <si>
-    <t>average no. of hours available for additional work in a week (0.0) for person with broad status in employment in CWS</t>
-  </si>
-  <si>
-    <t>percentage of workers available for additional work during the week for person with broad status in employment in CWS</t>
-  </si>
-  <si>
-    <t>Average wage/salary earnings (Rs.) during the preceding calendar month from regular wage/salaried  employment among the regular wage salaried employees</t>
-  </si>
-  <si>
     <t>no_days_worked</t>
   </si>
   <si>
@@ -367,9 +325,6 @@
   </si>
   <si>
     <t>Percentage distribution of workers</t>
-  </si>
-  <si>
-    <t>average no. of hours/ percentage of workers available for additional work</t>
   </si>
   <si>
     <t>Legislators, Senior Officials, and Managers</t>
@@ -418,61 +373,16 @@
 </t>
   </si>
   <si>
-    <t>24&lt;hours≤36</t>
-  </si>
-  <si>
-    <t>36&lt;hours≤48</t>
-  </si>
-  <si>
-    <t>48&lt;hours≤60</t>
-  </si>
-  <si>
-    <t>60&lt;hours≤72</t>
-  </si>
-  <si>
-    <t>72&lt;hours≤84</t>
-  </si>
-  <si>
-    <t>hours&gt; 84</t>
-  </si>
-  <si>
-    <t>sub_industry</t>
-  </si>
-  <si>
     <t>05-09 (mining &amp; quarrying)</t>
   </si>
   <si>
     <t>10-33 (manufacturing)</t>
   </si>
   <si>
-    <t>35-39 (electricity and  water supply)</t>
-  </si>
-  <si>
-    <t>41-43 (construction)</t>
-  </si>
-  <si>
-    <t>45-47 (trade)</t>
-  </si>
-  <si>
-    <t>49-53( transport)</t>
-  </si>
-  <si>
-    <t>55-56 (accommodation &amp; food services))</t>
-  </si>
-  <si>
-    <t>58-99 (other services)</t>
-  </si>
-  <si>
     <t>disaggregation_level</t>
   </si>
   <si>
     <t>proprietary_partnership</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>Public/  private  limited  company</t>
   </si>
   <si>
     <t xml:space="preserve">Proprietary and partnership
@@ -541,21 +451,6 @@
     <t>Number of hours actually worked  in a week</t>
   </si>
   <si>
-    <t>Trust/other non  profit inst</t>
-  </si>
-  <si>
-    <t>Autonom ous bodies</t>
-  </si>
-  <si>
-    <t>Govt./ local body/public sector enterprises</t>
-  </si>
-  <si>
-    <t>Proprietary and partnership</t>
-  </si>
-  <si>
-    <t>Usual Status (ps+ss)</t>
-  </si>
-  <si>
     <t>Rural</t>
   </si>
   <si>
@@ -636,6 +531,203 @@
   </si>
   <si>
     <t>Quarter</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>Hours&gt; 84</t>
+  </si>
+  <si>
+    <t>72&lt;Hours≤84</t>
+  </si>
+  <si>
+    <t>60&lt;Hours≤72</t>
+  </si>
+  <si>
+    <t>48&lt;Hours≤60</t>
+  </si>
+  <si>
+    <t>36&lt;Hours≤48</t>
+  </si>
+  <si>
+    <t>24&lt;Hours≤36</t>
+  </si>
+  <si>
+    <t>social_group</t>
+  </si>
+  <si>
+    <t>Scheduled Tribe</t>
+  </si>
+  <si>
+    <t>Scheduled Caste</t>
+  </si>
+  <si>
+    <t>Other backward classes</t>
+  </si>
+  <si>
+    <t>Average no. of hours/ percentage of workers available for additional work</t>
+  </si>
+  <si>
+    <t>Usual Status (PS + SS)</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>sub_self_employment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All self
+employed
+</t>
+  </si>
+  <si>
+    <t>Hinduism</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Christianity</t>
+  </si>
+  <si>
+    <t>Sikhism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By religious groups </t>
+  </si>
+  <si>
+    <t>By Social group</t>
+  </si>
+  <si>
+    <t>Autonomous Bodies</t>
+  </si>
+  <si>
+    <t>Govt./Local  Body/Public Sector Enterprises</t>
+  </si>
+  <si>
+    <t>Proprietary and Partnership</t>
+  </si>
+  <si>
+    <t>Employer’s Households</t>
+  </si>
+  <si>
+    <t>Trust/Other Non  Profit inst</t>
+  </si>
+  <si>
+    <t>Cooperative Societies</t>
+  </si>
+  <si>
+    <t>Public/ Private  Limited  Company</t>
+  </si>
+  <si>
+    <t>Labour Force Participation Rate</t>
+  </si>
+  <si>
+    <t>Worker Population Ratio</t>
+  </si>
+  <si>
+    <t>Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Average no. of days actually worked in a week (0.0) for person with broad status in employment in CWS</t>
+  </si>
+  <si>
+    <t>Average number of hours (0.0) actually worked per week considering all the economic activities performed during the week for person with broad status in employment in CWS</t>
+  </si>
+  <si>
+    <t>Average no. of days worked in a week (0.0) for person with broad status in employment in CWS</t>
+  </si>
+  <si>
+    <t>Average no. of hours available for additional work in a week (0.0) for person with broad status in employment in CWS</t>
+  </si>
+  <si>
+    <t>Percentage of workers available for additional work during the week for person with broad status in employment in CWS</t>
+  </si>
+  <si>
+    <t>umpce</t>
+  </si>
+  <si>
+    <t>0-10</t>
+  </si>
+  <si>
+    <t>10-20</t>
+  </si>
+  <si>
+    <t>20-30</t>
+  </si>
+  <si>
+    <t>30-40</t>
+  </si>
+  <si>
+    <t>40-50</t>
+  </si>
+  <si>
+    <t>50-60</t>
+  </si>
+  <si>
+    <t>60-70</t>
+  </si>
+  <si>
+    <t>70-80</t>
+  </si>
+  <si>
+    <t>80-90</t>
+  </si>
+  <si>
+    <t>90-100</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>for each decile class of Usual Monthly Per Capita Consumer Expenditure (UMPCE)</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>Average wage/salary earnings (Rs. 0.00) per day from casual labour work other than public works in CWS</t>
+  </si>
+  <si>
+    <t>01-03 (agriculture)</t>
+  </si>
+  <si>
+    <t>industry_nic_2</t>
+  </si>
+  <si>
+    <t>35-39 (electricity and  water supply)</t>
+  </si>
+  <si>
+    <t>41-43 (construction)</t>
+  </si>
+  <si>
+    <t>05-43 (secondary)</t>
+  </si>
+  <si>
+    <t>45-47 (trade)</t>
+  </si>
+  <si>
+    <t>49-53( transport)</t>
+  </si>
+  <si>
+    <t>55-56 (accommodation &amp; food services))</t>
+  </si>
+  <si>
+    <t>58-99 (other services)</t>
+  </si>
+  <si>
+    <t>45-99 (tertiary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total </t>
   </si>
 </sst>
 </file>
@@ -645,7 +737,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -667,12 +759,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -766,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -790,39 +876,69 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCF2A3A-443B-4F56-A389-6B42246D0AA4}">
-  <dimension ref="A1:AA38"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,16 +1279,21 @@
     <col min="16" max="16" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="51.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" customWidth="1"/>
+    <col min="23" max="23" width="23.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>39</v>
@@ -1187,699 +1308,804 @@
         <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="U2" t="s">
+        <v>163</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y2" s="29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="U3" t="s">
+        <v>164</v>
+      </c>
+      <c r="V3" t="s">
+        <v>184</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y3" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I4" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="R4" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="V4" t="s">
+        <v>185</v>
+      </c>
+      <c r="W4" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y4" s="29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="I5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" t="s">
+        <v>92</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="R5" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="T5" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="V5" t="s">
+        <v>186</v>
+      </c>
+      <c r="W5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y5" s="29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="O6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="R6" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="V6" t="s">
+        <v>110</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6" s="29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="O7" t="s">
+        <v>94</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="R7" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="S7" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="T7" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y7" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="L8" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" t="s">
+        <v>95</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q8" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="R8" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="S8" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y8" s="29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="R9" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="S9" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y9" s="29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="5" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="R1" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="P10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="R10" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="S10" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="T10" s="32"/>
+      <c r="Y10" s="29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="S11" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y11" s="29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="R12" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="S12" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="T2" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="U2" t="s">
-        <v>198</v>
-      </c>
-      <c r="AA2" s="23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="O3" t="s">
-        <v>104</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="Y12" s="34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="20"/>
+      <c r="R13" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="S13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="R4" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="T4" s="23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O5" t="s">
-        <v>106</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="T5" s="24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>181</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="M6" s="13"/>
-      <c r="O6" t="s">
-        <v>107</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q6" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="R6" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="C14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="O7" t="s">
-        <v>108</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q7" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="T7" s="23" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>183</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="O8" t="s">
-        <v>109</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="R8" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="T8" s="23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H9" s="9" t="s">
+    </row>
+    <row r="16" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="O9" t="s">
-        <v>110</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q9" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="R9" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="S9" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="T9" s="23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>185</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="P10" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q10" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="S10" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="T10" s="20"/>
-    </row>
-    <row r="11" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:27" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H17" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>75</v>
+      <c r="H18" s="20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>76</v>
+      <c r="H19" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>77</v>
+      <c r="H20" s="20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>78</v>
+      <c r="H21" s="20" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="22" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="15" t="s">
-        <v>196</v>
+      <c r="C38" s="12" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>